<commit_message>
BLACKLINE update 2025-05-31 14:05:17
</commit_message>
<xml_diff>
--- a/data/alertas_geopoliticas.xlsx
+++ b/data/alertas_geopoliticas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F139"/>
+  <dimension ref="A1:F189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4097,6 +4097,1306 @@
       </c>
       <c r="F139" t="inlineStr"/>
     </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Un aliado de la OTAN coge carrerilla con el avión 'invisible' que rivaliza con el supercaza de EEUU</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>military</t>
+        </is>
+      </c>
+      <c r="E140" t="n">
+        <v>2</v>
+      </c>
+      <c r="F140" t="inlineStr"/>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Un país clave de la OTAN pone en jaque a Rusia al revelar sus planes nucleares secretos</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E141" t="n">
+        <v>2</v>
+      </c>
+      <c r="F141" t="inlineStr"/>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Usan tierra de Fukushima en los canteros del primer ministro japonés para demostrar que no hay peligro</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E142" t="n">
+        <v>2</v>
+      </c>
+      <c r="F142" t="inlineStr"/>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Iberdrola asegura que en el apagón respondieron «siempre a los protocolos del Ministerio y de Redeia»</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E143" t="n">
+        <v>2</v>
+      </c>
+      <c r="F143" t="inlineStr"/>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Taco man</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E144" t="n">
+        <v>2</v>
+      </c>
+      <c r="F144" t="inlineStr"/>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Repsol llama a abandonar el "radicalismo ecologista" y reafirma su apuesta por los combustibles fósiles</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>2</v>
+      </c>
+      <c r="F145" t="inlineStr"/>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Galán señala a Aagesen y a Red Eléctrica en el apagón: "Iberdrola respondió según los protocolos"</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E146" t="n">
+        <v>2</v>
+      </c>
+      <c r="F146" t="inlineStr"/>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Zajárova: "Kiev quiere aumentar su valor con histeria pero solo le salen chichones"</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E147" t="n">
+        <v>2</v>
+      </c>
+      <c r="F147" t="inlineStr"/>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>La fabricante de los misiles nucleares intercontinentales regresa a la Luna para competir contra SpaceX</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E148" t="n">
+        <v>2</v>
+      </c>
+      <c r="F148" t="inlineStr"/>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Atomfall se despide por todo lo alto con Wicked Isle, su última expansión que llega en junio con nuevos enemigos, armas y finales</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E149" t="n">
+        <v>2</v>
+      </c>
+      <c r="F149" t="inlineStr"/>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>La guerra ya no es ficción: Algunos ya empezaron a desempolvar sus búnkeres y advierten que Europa vive una nueva era</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E150" t="n">
+        <v>2</v>
+      </c>
+      <c r="F150" t="inlineStr"/>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>El CCIB se prepara para acoger los grandes congresos médicos mundiales del año</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E151" t="n">
+        <v>2</v>
+      </c>
+      <c r="F151" t="inlineStr"/>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Si algo no necesitaba la guerra de Ucrania era el tema “nuclear”. Rusia lo acaba de activar, literalmente</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E152" t="n">
+        <v>2</v>
+      </c>
+      <c r="F152" t="inlineStr"/>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>La bandera fiscal a la que Mazón se aferra en medio de la tormenta</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E153" t="n">
+        <v>2</v>
+      </c>
+      <c r="F153" t="inlineStr"/>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Juegos para PC que corren en casi cualquier equipo</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E154" t="n">
+        <v>2</v>
+      </c>
+      <c r="F154" t="inlineStr"/>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Muere en un atentado en Rusia el militar al que Putin encargó el indiscriminado bombardeo de la ciudad de Mariúpol</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E155" t="n">
+        <v>2</v>
+      </c>
+      <c r="F155" t="inlineStr"/>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Por delante en tecnología, innovación y valores</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E156" t="n">
+        <v>2</v>
+      </c>
+      <c r="F156" t="inlineStr"/>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>El vecino de España da luz verde al plan de modernización para albergar bombarderos nucleares</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E157" t="n">
+        <v>2</v>
+      </c>
+      <c r="F157" t="inlineStr"/>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>¿El inicio de una guerra con Trump?</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E158" t="n">
+        <v>2</v>
+      </c>
+      <c r="F158" t="inlineStr"/>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Momentos "Eureka" decisivos en la historia de la Física</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E159" t="n">
+        <v>2</v>
+      </c>
+      <c r="F159" t="inlineStr"/>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Una empresa europea planea generar 100 MW durante 40 años a partir de residuos nucleares</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="E160" t="n">
+        <v>2</v>
+      </c>
+      <c r="F160" t="inlineStr"/>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>Hell is Us: Lo hemos jugado y os contamos que esperar de está nueva IP</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>drone</t>
+        </is>
+      </c>
+      <c r="E161" t="n">
+        <v>2</v>
+      </c>
+      <c r="F161" t="inlineStr"/>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Posibles anuncios de Summer Game Fest 2025: ¿Qué anunciarán compañías como Sony, Nintendo o Microsoft?</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>war</t>
+        </is>
+      </c>
+      <c r="E162" t="n">
+        <v>2</v>
+      </c>
+      <c r="F162" t="inlineStr"/>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>La temporada 4 de 'Bleach TYBW' promete ser tremenda, pero tiene al propio Tite Kubo preocupado por el final del anime</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>war</t>
+        </is>
+      </c>
+      <c r="E163" t="n">
+        <v>2</v>
+      </c>
+      <c r="F163" t="inlineStr"/>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>'Something beautiful': el nuevo disco de Miley Cyrus suena a todo y a nada a la vez</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>war</t>
+        </is>
+      </c>
+      <c r="E164" t="n">
+        <v>2</v>
+      </c>
+      <c r="F164" t="inlineStr"/>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>La película de ‘Elden Ring’ quiere a esta estrella de Netflix y ‘Warfare’ como protagonista</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>war</t>
+        </is>
+      </c>
+      <c r="E165" t="n">
+        <v>2</v>
+      </c>
+      <c r="F165" t="inlineStr"/>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Corcuera y Arabia: esta es la fascinante historia de las dos mujeres españolas que formaron parte del ejército americano durante la Segunda Guerra Mundial</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>war</t>
+        </is>
+      </c>
+      <c r="E166" t="n">
+        <v>2</v>
+      </c>
+      <c r="F166" t="inlineStr"/>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>‘Something Beautiful’ de Miley Cyrus: algo bonito y seguro</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>war</t>
+        </is>
+      </c>
+      <c r="E167" t="n">
+        <v>2</v>
+      </c>
+      <c r="F167" t="inlineStr"/>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Se filtra un nuevo juego que va camino de Nintendo Switch 2. Un espectáculo gráfico que nos tiene a muchos muy intrigados</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>war</t>
+        </is>
+      </c>
+      <c r="E168" t="n">
+        <v>2</v>
+      </c>
+      <c r="F168" t="inlineStr"/>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>El director de la película Elden Ring ya tiene algunas ideas para el reparto</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>war</t>
+        </is>
+      </c>
+      <c r="E169" t="n">
+        <v>2</v>
+      </c>
+      <c r="F169" t="inlineStr"/>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Adiós al examen teórico de toda la vida: la DGT planea cambios radicales en el test con vídeos y respuestas mútiples</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E170" t="n">
+        <v>2</v>
+      </c>
+      <c r="F170" t="inlineStr"/>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>¡Estamos en problemas! Dos de las peores termitas del mundo se han cruzado en Florida.</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E171" t="n">
+        <v>2</v>
+      </c>
+      <c r="F171" t="inlineStr"/>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Habrá otra spinoff para TV de «The Batman»</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E172" t="n">
+        <v>2</v>
+      </c>
+      <c r="F172" t="inlineStr"/>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>Una uruguaya que vive en España impresionada por el dinero que se paga por ir a una boda en nuestro país: «El verdadero terror debe ser...»</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E173" t="n">
+        <v>2</v>
+      </c>
+      <c r="F173" t="inlineStr"/>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>'Elden Ring': Kit Connor suena para protagonizar el live-action del videojuego dirigido por Alex Garland</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E174" t="n">
+        <v>2</v>
+      </c>
+      <c r="F174" t="inlineStr"/>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Coca-Cola devuelve más agua de la que consume</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E175" t="n">
+        <v>2</v>
+      </c>
+      <c r="F175" t="inlineStr"/>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Otrora signos de terror, los cometas revelan ahora secretos del universo</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E176" t="n">
+        <v>2</v>
+      </c>
+      <c r="F176" t="inlineStr"/>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Top juegos indie imprescindibles para PC</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E177" t="n">
+        <v>2</v>
+      </c>
+      <c r="F177" t="inlineStr"/>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Five Nights at Freddy's se va del streaming</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E178" t="n">
+        <v>2</v>
+      </c>
+      <c r="F178" t="inlineStr"/>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Planes familiares para el último fin de semana de mayo... y primero de junio</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E179" t="n">
+        <v>2</v>
+      </c>
+      <c r="F179" t="inlineStr"/>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>¿Está La calle del terror: La reina del baile basada en hechos reales?</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E180" t="n">
+        <v>2</v>
+      </c>
+      <c r="F180" t="inlineStr"/>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Primer piso de espanto</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E181" t="n">
+        <v>2</v>
+      </c>
+      <c r="F181" t="inlineStr"/>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>No solo Grupo Fugitivo: El Cártel del Golfo arrastra un historial de matanzas desde hace más de 40 años</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E182" t="n">
+        <v>2</v>
+      </c>
+      <c r="F182" t="inlineStr"/>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>Wes Anderson vuelve tan simétrico como siempre tras salir escaldado de Cannes. Lo mejor y lo peor de los estrenos de cine</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E183" t="n">
+        <v>2</v>
+      </c>
+      <c r="F183" t="inlineStr"/>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>Todos los nuevos juegos que llegan a Xbox para cerrar mayo por todo lo alto</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E184" t="n">
+        <v>2</v>
+      </c>
+      <c r="F184" t="inlineStr"/>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>Guía para disfrutar el Sundance Film Festival CDMX 2025: sedes, películas y boletos</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E185" t="n">
+        <v>2</v>
+      </c>
+      <c r="F185" t="inlineStr"/>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>Por el honor y 330 mil dólares: Colo Colo cierra su Copa Libertadores más amarga venciendo al rústico Bucaramanga</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E186" t="n">
+        <v>2</v>
+      </c>
+      <c r="F186" t="inlineStr"/>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>Estado Islámico ataca por primera vez a los sucesores de Bashar al Asad</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E187" t="n">
+        <v>2</v>
+      </c>
+      <c r="F187" t="inlineStr"/>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>Ángel Di María, ante el desafío de romper una nueva pared: ahora, con Rosario Central</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>terror</t>
+        </is>
+      </c>
+      <c r="E188" t="n">
+        <v>2</v>
+      </c>
+      <c r="F188" t="inlineStr"/>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Desconocido</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Todos los juegos de lanzamiento de Switch 2 con los que podrás estrenar la consola de Nintendo</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>attack</t>
+        </is>
+      </c>
+      <c r="E189" t="n">
+        <v>2</v>
+      </c>
+      <c r="F189" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>